<commit_message>
yeongsanggang 2020 -< 6/4
</commit_message>
<xml_diff>
--- a/data/yeong/수질/광산_2020.xlsx
+++ b/data/yeong/수질/광산_2020.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\사업관련\환경AI\모듈작업\water-quality\data\yeong\수질\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="122">
   <si>
     <t>dt</t>
   </si>
@@ -378,131 +385,37 @@
   </si>
   <si>
     <t>20200525</t>
-  </si>
-  <si>
-    <t>2020-06-06 12:00</t>
-  </si>
-  <si>
-    <t>20200601</t>
-  </si>
-  <si>
-    <t>2020-06-12 12:00</t>
-  </si>
-  <si>
-    <t>20200608</t>
-  </si>
-  <si>
-    <t>2020-06-18 12:00</t>
-  </si>
-  <si>
-    <t>20200615</t>
-  </si>
-  <si>
-    <t>2020-06-24 12:00</t>
-  </si>
-  <si>
-    <t>20200622</t>
-  </si>
-  <si>
-    <t>2020-07-05 12:00</t>
-  </si>
-  <si>
-    <t>20200701</t>
-  </si>
-  <si>
-    <t>2020-07-10 12:00</t>
-  </si>
-  <si>
-    <t>20200706</t>
-  </si>
-  <si>
-    <t>2020-07-15 12:00</t>
-  </si>
-  <si>
-    <t>20200715</t>
-  </si>
-  <si>
-    <t>2020-07-20 12:00</t>
-  </si>
-  <si>
-    <t>20200721</t>
-  </si>
-  <si>
-    <t>2020-07-25 12:00</t>
-  </si>
-  <si>
-    <t>20200727</t>
-  </si>
-  <si>
-    <t>2020-08-08 12:00</t>
-  </si>
-  <si>
-    <t>20200803</t>
-  </si>
-  <si>
-    <t>2020-08-16 12:00</t>
-  </si>
-  <si>
-    <t>20200819</t>
-  </si>
-  <si>
-    <t>2020-08-24 12:00</t>
-  </si>
-  <si>
-    <t>20200824</t>
-  </si>
-  <si>
-    <t>2020-09-05 12:00</t>
-  </si>
-  <si>
-    <t>20200901</t>
-  </si>
-  <si>
-    <t>2020-09-10 12:00</t>
-  </si>
-  <si>
-    <t>20200908</t>
-  </si>
-  <si>
-    <t>2020-09-15 12:00</t>
-  </si>
-  <si>
-    <t>20200914</t>
-  </si>
-  <si>
-    <t>2020-09-20 12:00</t>
-  </si>
-  <si>
-    <t>20200921</t>
-  </si>
-  <si>
-    <t>2020-09-25 12:00</t>
-  </si>
-  <si>
-    <t>20200928</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="0.000000"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="176" formatCode="0.000000"/>
+    <numFmt numFmtId="177" formatCode="0.000"/>
+    <numFmt numFmtId="178" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -520,7 +433,13 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -528,16 +447,24 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -546,10 +473,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -795,83 +722,81 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
+  <dimension ref="A1:BJ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.44" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.56" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.78" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.78" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.89" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.56" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.44" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.22" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.33" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.56" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.33" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.56" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.33" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.56" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.33" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.56" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.33" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.56" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.33" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.56" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.22" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.33" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.56" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.33" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.33" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.33" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="4.11" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.22" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="4.78" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.11" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="5.22" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="5.22" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="6.33" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="6.33" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.56" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="5.22" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="13.22" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="6.33" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.33" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="6.33" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="4.44" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="10.78" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="10.78" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="8.44" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="9.44" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="8.11" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="9.67" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="7.78" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.44" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="8" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="8" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="9.67" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="9.56" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="17.78" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="10.78" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="9.22" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="9.22" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="4.125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="4.75" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="42" max="44" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="46" max="47" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="54" max="55" width="8" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="9.25" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1059,7 +984,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -1139,13 +1064,13 @@
         <v>3.4649999999999999</v>
       </c>
       <c r="AD2" s="4">
-        <v>3.5099999999999998</v>
+        <v>3.51</v>
       </c>
       <c r="AE2" s="5">
         <v>7.5</v>
       </c>
       <c r="AF2" s="5">
-        <v>9.5999999999999996</v>
+        <v>9.6</v>
       </c>
       <c r="AG2">
         <v>439</v>
@@ -1160,10 +1085,10 @@
         <v>13.5</v>
       </c>
       <c r="AK2" s="4">
-        <v>7.7400000000000002</v>
+        <v>7.74</v>
       </c>
       <c r="AL2" s="3">
-        <v>0.087999999999999995</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="AM2" s="3">
         <v>9.7629999999999999</v>
@@ -1172,7 +1097,7 @@
         <v>7.5</v>
       </c>
       <c r="AO2" s="5">
-        <v>69.700000000000003</v>
+        <v>69.7</v>
       </c>
       <c r="AP2">
         <v>0</v>
@@ -1181,13 +1106,13 @@
         <v>7.6559999999999997</v>
       </c>
       <c r="AR2" s="3">
-        <v>0.014999999999999999</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="AS2" s="5">
-        <v>8.5999999999999996</v>
+        <v>8.6</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -1270,10 +1195,10 @@
         <v>2.911</v>
       </c>
       <c r="AE3" s="5">
-        <v>7.2999999999999998</v>
+        <v>7.3</v>
       </c>
       <c r="AF3" s="5">
-        <v>7.2000000000000002</v>
+        <v>7.2</v>
       </c>
       <c r="AG3">
         <v>280</v>
@@ -1303,19 +1228,19 @@
         <v>16.899999999999999</v>
       </c>
       <c r="AP3" s="3">
-        <v>0.036999999999999998</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="AQ3" s="3">
         <v>5.0309999999999997</v>
       </c>
       <c r="AR3" s="3">
-        <v>0.055</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AS3" s="5">
-        <v>5.4000000000000004</v>
+        <v>5.4</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>81</v>
       </c>
@@ -1398,10 +1323,10 @@
         <v>3.641</v>
       </c>
       <c r="AE4" s="5">
-        <v>7.2000000000000002</v>
+        <v>7.2</v>
       </c>
       <c r="AF4" s="5">
-        <v>7.4000000000000004</v>
+        <v>7.4</v>
       </c>
       <c r="AG4">
         <v>364</v>
@@ -1410,40 +1335,40 @@
         <v>4</v>
       </c>
       <c r="AI4" s="5">
-        <v>7.4000000000000004</v>
+        <v>7.4</v>
       </c>
       <c r="AJ4" s="5">
-        <v>10.300000000000001</v>
+        <v>10.3</v>
       </c>
       <c r="AK4" s="3">
         <v>6.702</v>
       </c>
       <c r="AL4" s="3">
-        <v>0.094</v>
+        <v>9.4E-2</v>
       </c>
       <c r="AM4" s="3">
         <v>10.532999999999999</v>
       </c>
       <c r="AN4" s="5">
-        <v>6.7999999999999998</v>
+        <v>6.8</v>
       </c>
       <c r="AO4" s="5">
-        <v>20.899999999999999</v>
+        <v>20.9</v>
       </c>
       <c r="AP4" s="4">
-        <v>0.029999999999999999</v>
+        <v>0.03</v>
       </c>
       <c r="AQ4" s="3">
         <v>6.4409999999999998</v>
       </c>
       <c r="AR4" s="3">
-        <v>0.042000000000000003</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="AS4" s="5">
-        <v>5.9000000000000004</v>
+        <v>5.9</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>84</v>
       </c>
@@ -1526,16 +1451,16 @@
         <v>2.931</v>
       </c>
       <c r="AE5" s="5">
-        <v>7.2000000000000002</v>
+        <v>7.2</v>
       </c>
       <c r="AF5" s="5">
-        <v>7.7999999999999998</v>
+        <v>7.8</v>
       </c>
       <c r="AG5">
         <v>362</v>
       </c>
       <c r="AH5" s="5">
-        <v>4.7999999999999998</v>
+        <v>4.8</v>
       </c>
       <c r="AI5" s="5">
         <v>8.3000000000000007</v>
@@ -1556,22 +1481,22 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="AO5" s="5">
-        <v>21.399999999999999</v>
+        <v>21.4</v>
       </c>
       <c r="AP5" s="3">
-        <v>0.032000000000000001</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="AQ5" s="3">
         <v>6.891</v>
       </c>
       <c r="AR5" s="3">
-        <v>0.048000000000000001</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="AS5" s="5">
-        <v>6.2999999999999998</v>
+        <v>6.3</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -1648,22 +1573,22 @@
         <v>88</v>
       </c>
       <c r="AC6" s="4">
-        <v>2.9700000000000002</v>
+        <v>2.97</v>
       </c>
       <c r="AD6" s="3">
         <v>2.605</v>
       </c>
       <c r="AE6" s="5">
-        <v>7.2000000000000002</v>
+        <v>7.2</v>
       </c>
       <c r="AF6" s="5">
-        <v>8.9000000000000004</v>
+        <v>8.9</v>
       </c>
       <c r="AG6">
         <v>380</v>
       </c>
       <c r="AH6" s="5">
-        <v>5.7000000000000002</v>
+        <v>5.7</v>
       </c>
       <c r="AI6" s="5">
         <v>11.1</v>
@@ -1678,28 +1603,28 @@
         <v>0.105</v>
       </c>
       <c r="AM6" s="5">
-        <v>13.199999999999999</v>
+        <v>13.2</v>
       </c>
       <c r="AN6" s="5">
-        <v>8.5999999999999996</v>
+        <v>8.6</v>
       </c>
       <c r="AO6" s="5">
-        <v>28.300000000000001</v>
+        <v>28.3</v>
       </c>
       <c r="AP6" s="3">
-        <v>0.063</v>
+        <v>6.3E-2</v>
       </c>
       <c r="AQ6" s="3">
         <v>5.5810000000000004</v>
       </c>
       <c r="AR6" s="3">
-        <v>0.076999999999999999</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="AS6" s="5">
-        <v>7.2999999999999998</v>
+        <v>7.3</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>89</v>
       </c>
@@ -1782,7 +1707,7 @@
         <v>3.9169999999999998</v>
       </c>
       <c r="AE7" s="5">
-        <v>7.2999999999999998</v>
+        <v>7.3</v>
       </c>
       <c r="AF7" s="5">
         <v>8.5</v>
@@ -1794,7 +1719,7 @@
         <v>5.5</v>
       </c>
       <c r="AI7" s="5">
-        <v>7.2999999999999998</v>
+        <v>7.3</v>
       </c>
       <c r="AJ7" s="5">
         <v>12.1</v>
@@ -1803,31 +1728,31 @@
         <v>7.367</v>
       </c>
       <c r="AL7" s="4">
-        <v>0.080000000000000002</v>
+        <v>0.08</v>
       </c>
       <c r="AM7" s="4">
-        <v>7.8300000000000001</v>
+        <v>7.83</v>
       </c>
       <c r="AN7" s="5">
-        <v>6.9000000000000004</v>
+        <v>6.9</v>
       </c>
       <c r="AO7">
         <v>24</v>
       </c>
       <c r="AP7" s="3">
-        <v>0.014</v>
+        <v>1.4E-2</v>
       </c>
       <c r="AQ7" s="3">
         <v>7.2359999999999998</v>
       </c>
       <c r="AR7" s="3">
-        <v>0.029000000000000001</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="AS7" s="5">
-        <v>6.9000000000000004</v>
+        <v>6.9</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>91</v>
       </c>
@@ -1910,7 +1835,7 @@
         <v>2.2730000000000001</v>
       </c>
       <c r="AE8" s="5">
-        <v>7.4000000000000004</v>
+        <v>7.4</v>
       </c>
       <c r="AF8" s="5">
         <v>12.9</v>
@@ -1919,10 +1844,10 @@
         <v>365</v>
       </c>
       <c r="AH8" s="5">
-        <v>6.7999999999999998</v>
+        <v>6.8</v>
       </c>
       <c r="AI8" s="5">
-        <v>15.199999999999999</v>
+        <v>15.2</v>
       </c>
       <c r="AJ8" s="5">
         <v>10.199999999999999</v>
@@ -1931,13 +1856,13 @@
         <v>6.7279999999999998</v>
       </c>
       <c r="AL8" s="4">
-        <v>0.27000000000000002</v>
+        <v>0.27</v>
       </c>
       <c r="AN8" s="5">
-        <v>7.7000000000000002</v>
+        <v>7.7</v>
       </c>
       <c r="AO8" s="5">
-        <v>45.299999999999997</v>
+        <v>45.3</v>
       </c>
       <c r="AP8" s="4">
         <v>0.11</v>
@@ -1949,10 +1874,10 @@
         <v>0.14699999999999999</v>
       </c>
       <c r="AS8" s="5">
-        <v>7.4000000000000004</v>
+        <v>7.4</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>93</v>
       </c>
@@ -2065,7 +1990,7 @@
         <v>10.199999999999999</v>
       </c>
       <c r="AO9" s="5">
-        <v>57.399999999999999</v>
+        <v>57.4</v>
       </c>
       <c r="AP9" s="3">
         <v>0.152</v>
@@ -2080,7 +2005,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -2163,10 +2088,10 @@
         <v>2.1440000000000001</v>
       </c>
       <c r="AE10" s="5">
-        <v>7.5999999999999996</v>
+        <v>7.6</v>
       </c>
       <c r="AF10" s="5">
-        <v>7.9000000000000004</v>
+        <v>7.9</v>
       </c>
       <c r="AG10">
         <v>317</v>
@@ -2178,7 +2103,7 @@
         <v>13.6</v>
       </c>
       <c r="AJ10" s="5">
-        <v>11.199999999999999</v>
+        <v>11.2</v>
       </c>
       <c r="AK10" s="3">
         <v>4.5069999999999997</v>
@@ -2193,22 +2118,22 @@
         <v>10.199999999999999</v>
       </c>
       <c r="AO10" s="5">
-        <v>27.899999999999999</v>
+        <v>27.9</v>
       </c>
       <c r="AP10" s="3">
-        <v>0.029000000000000001</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="AQ10" s="3">
         <v>4.4930000000000003</v>
       </c>
       <c r="AR10" s="3">
-        <v>0.043999999999999997</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="AS10">
         <v>6</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>97</v>
       </c>
@@ -2285,13 +2210,13 @@
         <v>98</v>
       </c>
       <c r="AC11" s="4">
-        <v>3.5800000000000001</v>
+        <v>3.58</v>
       </c>
       <c r="AD11" s="3">
         <v>2.698</v>
       </c>
       <c r="AE11" s="5">
-        <v>7.0999999999999996</v>
+        <v>7.1</v>
       </c>
       <c r="AF11">
         <v>9</v>
@@ -2312,31 +2237,31 @@
         <v>7.1349999999999998</v>
       </c>
       <c r="AL11" s="4">
-        <v>0.14999999999999999</v>
+        <v>0.15</v>
       </c>
       <c r="AM11" s="3">
         <v>15.254</v>
       </c>
       <c r="AN11" s="5">
-        <v>11.300000000000001</v>
+        <v>11.3</v>
       </c>
       <c r="AO11" s="5">
         <v>31.5</v>
       </c>
       <c r="AP11" s="3">
-        <v>0.010999999999999999</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="AQ11" s="3">
         <v>6.6429999999999998</v>
       </c>
       <c r="AR11" s="3">
-        <v>0.037999999999999999</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="AS11" s="5">
-        <v>7.4000000000000004</v>
+        <v>7.4</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>99</v>
       </c>
@@ -2419,7 +2344,7 @@
         <v>2.5459999999999998</v>
       </c>
       <c r="AE12" s="5">
-        <v>7.5999999999999996</v>
+        <v>7.6</v>
       </c>
       <c r="AF12" s="5">
         <v>12.6</v>
@@ -2428,7 +2353,7 @@
         <v>392</v>
       </c>
       <c r="AH12" s="5">
-        <v>6.5999999999999996</v>
+        <v>6.6</v>
       </c>
       <c r="AI12">
         <v>19</v>
@@ -2449,22 +2374,22 @@
         <v>11.1</v>
       </c>
       <c r="AO12" s="5">
-        <v>88.400000000000006</v>
+        <v>88.4</v>
       </c>
       <c r="AP12" s="3">
-        <v>0.0050000000000000001</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AQ12" s="3">
         <v>6.6769999999999996</v>
       </c>
       <c r="AR12" s="3">
-        <v>0.032000000000000001</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="AS12" s="5">
-        <v>8.4000000000000004</v>
+        <v>8.4</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>101</v>
       </c>
@@ -2550,7 +2475,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="AF13" s="5">
-        <v>13.699999999999999</v>
+        <v>13.7</v>
       </c>
       <c r="AG13">
         <v>431</v>
@@ -2574,25 +2499,25 @@
         <v>7.2309999999999999</v>
       </c>
       <c r="AN13" s="5">
-        <v>14.699999999999999</v>
+        <v>14.7</v>
       </c>
       <c r="AO13" s="5">
         <v>107.3</v>
       </c>
       <c r="AP13" s="3">
-        <v>0.0040000000000000001</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="AQ13" s="3">
         <v>6.6150000000000002</v>
       </c>
       <c r="AR13" s="3">
-        <v>0.029000000000000001</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="AS13" s="5">
-        <v>8.0999999999999996</v>
+        <v>8.1</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>103</v>
       </c>
@@ -2675,7 +2600,7 @@
         <v>1.538</v>
       </c>
       <c r="AE14" s="5">
-        <v>7.2999999999999998</v>
+        <v>7.3</v>
       </c>
       <c r="AF14" s="5">
         <v>12.5</v>
@@ -2699,13 +2624,13 @@
         <v>0.23699999999999999</v>
       </c>
       <c r="AM14" s="5">
-        <v>13.199999999999999</v>
+        <v>13.2</v>
       </c>
       <c r="AN14" s="5">
-        <v>13.199999999999999</v>
+        <v>13.2</v>
       </c>
       <c r="AO14" s="5">
-        <v>121.59999999999999</v>
+        <v>121.6</v>
       </c>
       <c r="AP14" s="4">
         <v>0.01</v>
@@ -2714,13 +2639,13 @@
         <v>4.4390000000000001</v>
       </c>
       <c r="AR14" s="3">
-        <v>0.042000000000000003</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="AS14" s="5">
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>106</v>
       </c>
@@ -2797,7 +2722,7 @@
         <v>107</v>
       </c>
       <c r="AC15" s="4">
-        <v>2.6200000000000001</v>
+        <v>2.62</v>
       </c>
       <c r="AD15" s="3">
         <v>2.8290000000000002</v>
@@ -2806,7 +2731,7 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="AF15" s="5">
-        <v>15.800000000000001</v>
+        <v>15.8</v>
       </c>
       <c r="AG15">
         <v>419</v>
@@ -2815,10 +2740,10 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="AI15" s="5">
-        <v>23.699999999999999</v>
+        <v>23.7</v>
       </c>
       <c r="AJ15" s="5">
-        <v>16.300000000000001</v>
+        <v>16.3</v>
       </c>
       <c r="AK15" s="3">
         <v>6.3540000000000001</v>
@@ -2833,22 +2758,22 @@
         <v>14.4</v>
       </c>
       <c r="AO15" s="5">
-        <v>120.90000000000001</v>
+        <v>120.9</v>
       </c>
       <c r="AP15" s="3">
-        <v>0.0040000000000000001</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="AQ15" s="3">
         <v>6.202</v>
       </c>
       <c r="AR15" s="3">
-        <v>0.033000000000000002</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="AS15" s="5">
-        <v>9.5999999999999996</v>
+        <v>9.6</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>108</v>
       </c>
@@ -2931,7 +2856,7 @@
         <v>3.177</v>
       </c>
       <c r="AE16" s="5">
-        <v>7.2999999999999998</v>
+        <v>7.3</v>
       </c>
       <c r="AF16" s="5">
         <v>12.9</v>
@@ -2940,19 +2865,19 @@
         <v>469</v>
       </c>
       <c r="AH16" s="5">
-        <v>6.7999999999999998</v>
+        <v>6.8</v>
       </c>
       <c r="AI16">
         <v>14</v>
       </c>
       <c r="AJ16" s="5">
-        <v>10.699999999999999</v>
+        <v>10.7</v>
       </c>
       <c r="AK16" s="3">
         <v>8.7759999999999998</v>
       </c>
       <c r="AL16" s="3">
-        <v>0.088999999999999996</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="AM16" s="5">
         <v>10.6</v>
@@ -2961,22 +2886,22 @@
         <v>14.6</v>
       </c>
       <c r="AO16" s="5">
-        <v>61.399999999999999</v>
+        <v>61.4</v>
       </c>
       <c r="AP16" s="3">
-        <v>0.012999999999999999</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="AQ16" s="3">
         <v>8.7170000000000005</v>
       </c>
       <c r="AR16" s="3">
-        <v>0.058999999999999997</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="AS16" s="5">
-        <v>8.0999999999999996</v>
+        <v>8.1</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>110</v>
       </c>
@@ -3059,22 +2984,22 @@
         <v>1.046</v>
       </c>
       <c r="AE17" s="5">
-        <v>6.7999999999999998</v>
+        <v>6.8</v>
       </c>
       <c r="AF17" s="5">
-        <v>13.199999999999999</v>
+        <v>13.2</v>
       </c>
       <c r="AG17">
         <v>326</v>
       </c>
       <c r="AH17" s="5">
-        <v>7.5999999999999996</v>
+        <v>7.6</v>
       </c>
       <c r="AI17" s="5">
         <v>18.5</v>
       </c>
       <c r="AJ17" s="5">
-        <v>3.3999999999999999</v>
+        <v>3.4</v>
       </c>
       <c r="AK17" s="3">
         <v>7.3049999999999997</v>
@@ -3104,7 +3029,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>112</v>
       </c>
@@ -3187,10 +3112,10 @@
         <v>2.5049999999999999</v>
       </c>
       <c r="AE18" s="5">
-        <v>7.9000000000000004</v>
+        <v>7.9</v>
       </c>
       <c r="AF18" s="5">
-        <v>14.800000000000001</v>
+        <v>14.8</v>
       </c>
       <c r="AG18">
         <v>412</v>
@@ -3202,7 +3127,7 @@
         <v>16.399999999999999</v>
       </c>
       <c r="AJ18" s="5">
-        <v>13.699999999999999</v>
+        <v>13.7</v>
       </c>
       <c r="AK18" s="3">
         <v>7.056</v>
@@ -3217,22 +3142,22 @@
         <v>16.5</v>
       </c>
       <c r="AO18" s="5">
-        <v>60.899999999999999</v>
+        <v>60.9</v>
       </c>
       <c r="AP18" s="3">
-        <v>0.0050000000000000001</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AQ18" s="3">
         <v>6.5590000000000002</v>
       </c>
       <c r="AR18" s="3">
-        <v>0.036999999999999998</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="AS18" s="5">
-        <v>8.9000000000000004</v>
+        <v>8.9</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>114</v>
       </c>
@@ -3315,7 +3240,7 @@
         <v>1.2010000000000001</v>
       </c>
       <c r="AE19" s="5">
-        <v>6.7000000000000002</v>
+        <v>6.7</v>
       </c>
       <c r="AF19" s="5">
         <v>12.1</v>
@@ -3327,10 +3252,10 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="AI19" s="5">
-        <v>16.800000000000001</v>
+        <v>16.8</v>
       </c>
       <c r="AJ19" s="5">
-        <v>1.6000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="AK19" s="3">
         <v>6.6550000000000002</v>
@@ -3348,7 +3273,7 @@
         <v>14</v>
       </c>
       <c r="AP19" s="3">
-        <v>0.098000000000000004</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="AQ19" s="3">
         <v>5.835</v>
@@ -3360,7 +3285,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>116</v>
       </c>
@@ -3452,13 +3377,13 @@
         <v>290</v>
       </c>
       <c r="AH20" s="5">
-        <v>6.2999999999999998</v>
+        <v>6.3</v>
       </c>
       <c r="AI20" s="5">
-        <v>7.9000000000000004</v>
+        <v>7.9</v>
       </c>
       <c r="AJ20" s="5">
-        <v>4.2000000000000002</v>
+        <v>4.2</v>
       </c>
       <c r="AK20" s="3">
         <v>3.7389999999999999</v>
@@ -3473,7 +3398,7 @@
         <v>19.399999999999999</v>
       </c>
       <c r="AO20" s="5">
-        <v>26.300000000000001</v>
+        <v>26.3</v>
       </c>
       <c r="AP20" s="3">
         <v>0.108</v>
@@ -3485,10 +3410,10 @@
         <v>0.13700000000000001</v>
       </c>
       <c r="AS20" s="5">
-        <v>7.0999999999999996</v>
+        <v>7.1</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>118</v>
       </c>
@@ -3571,7 +3496,7 @@
         <v>0.97499999999999998</v>
       </c>
       <c r="AE21" s="5">
-        <v>6.7999999999999998</v>
+        <v>6.8</v>
       </c>
       <c r="AF21" s="5">
         <v>12.1</v>
@@ -3580,7 +3505,7 @@
         <v>293</v>
       </c>
       <c r="AH21" s="5">
-        <v>6.7000000000000002</v>
+        <v>6.7</v>
       </c>
       <c r="AI21" s="5">
         <v>11.5</v>
@@ -3598,25 +3523,25 @@
         <v>22.786999999999999</v>
       </c>
       <c r="AN21" s="5">
-        <v>21.199999999999999</v>
+        <v>21.2</v>
       </c>
       <c r="AO21" s="5">
         <v>66.5</v>
       </c>
       <c r="AP21" s="4">
-        <v>0.040000000000000001</v>
+        <v>0.04</v>
       </c>
       <c r="AQ21" s="3">
         <v>3.294</v>
       </c>
       <c r="AR21" s="3">
-        <v>0.069000000000000006</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="AS21" s="5">
-        <v>7.9000000000000004</v>
+        <v>7.9</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>120</v>
       </c>
@@ -3699,7 +3624,7 @@
         <v>1.6479999999999999</v>
       </c>
       <c r="AE22" s="5">
-        <v>6.9000000000000004</v>
+        <v>6.9</v>
       </c>
       <c r="AF22" s="5">
         <v>10.199999999999999</v>
@@ -3714,7 +3639,7 @@
         <v>17.600000000000001</v>
       </c>
       <c r="AJ22" s="5">
-        <v>6.7999999999999998</v>
+        <v>6.8</v>
       </c>
       <c r="AK22" s="3">
         <v>5.2729999999999997</v>
@@ -3726,2201 +3651,26 @@
         <v>19.356000000000002</v>
       </c>
       <c r="AN22" s="5">
-        <v>21.600000000000001</v>
+        <v>21.6</v>
       </c>
       <c r="AO22" s="5">
         <v>58.5</v>
       </c>
       <c r="AP22" s="3">
-        <v>0.028000000000000001</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="AQ22" s="3">
         <v>4.9569999999999999</v>
       </c>
       <c r="AR22" s="3">
-        <v>0.051999999999999998</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="AS22" s="5">
-        <v>7.0999999999999996</v>
+        <v>7.1</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>122</v>
-      </c>
-      <c r="B23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" t="s">
-        <v>65</v>
-      </c>
-      <c r="E23" s="2">
-        <v>35.062860999999998</v>
-      </c>
-      <c r="F23" s="2">
-        <v>126.772972</v>
-      </c>
-      <c r="G23" t="s">
-        <v>66</v>
-      </c>
-      <c r="H23" t="s">
-        <v>67</v>
-      </c>
-      <c r="L23" t="s">
-        <v>66</v>
-      </c>
-      <c r="M23" t="s">
-        <v>67</v>
-      </c>
-      <c r="N23" t="s">
-        <v>68</v>
-      </c>
-      <c r="O23" t="s">
-        <v>69</v>
-      </c>
-      <c r="P23" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>71</v>
-      </c>
-      <c r="R23" t="s">
-        <v>72</v>
-      </c>
-      <c r="S23" t="s">
-        <v>73</v>
-      </c>
-      <c r="T23" t="s">
-        <v>74</v>
-      </c>
-      <c r="U23" t="s">
-        <v>75</v>
-      </c>
-      <c r="V23" t="s">
-        <v>68</v>
-      </c>
-      <c r="W23" t="s">
-        <v>69</v>
-      </c>
-      <c r="X23" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA23" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>123</v>
-      </c>
-      <c r="AC23" s="3">
-        <v>2.5019999999999998</v>
-      </c>
-      <c r="AD23" s="4">
-        <v>1.3899999999999999</v>
-      </c>
-      <c r="AE23" s="5">
-        <v>6.9000000000000004</v>
-      </c>
-      <c r="AF23" s="5">
-        <v>10.1</v>
-      </c>
-      <c r="AG23">
-        <v>346</v>
-      </c>
-      <c r="AH23">
-        <v>6</v>
-      </c>
-      <c r="AI23" s="5">
-        <v>10.699999999999999</v>
-      </c>
-      <c r="AJ23" s="5">
-        <v>6.7000000000000002</v>
-      </c>
-      <c r="AK23" s="3">
-        <v>4.8789999999999996</v>
-      </c>
-      <c r="AL23" s="3">
-        <v>0.11600000000000001</v>
-      </c>
-      <c r="AM23" s="3">
-        <v>26.277000000000001</v>
-      </c>
-      <c r="AN23" s="5">
-        <v>22.899999999999999</v>
-      </c>
-      <c r="AO23" s="5">
-        <v>38.100000000000001</v>
-      </c>
-      <c r="AP23" s="3">
-        <v>0.025999999999999999</v>
-      </c>
-      <c r="AQ23" s="3">
-        <v>4.6050000000000004</v>
-      </c>
-      <c r="AR23" s="3">
-        <v>0.050999999999999997</v>
-      </c>
-      <c r="AS23" s="5">
-        <v>6.4000000000000004</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>124</v>
-      </c>
-      <c r="B24" t="s">
-        <v>79</v>
-      </c>
-      <c r="C24" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" t="s">
-        <v>65</v>
-      </c>
-      <c r="E24" s="2">
-        <v>35.062860999999998</v>
-      </c>
-      <c r="F24" s="2">
-        <v>126.772972</v>
-      </c>
-      <c r="G24" t="s">
-        <v>66</v>
-      </c>
-      <c r="H24" t="s">
-        <v>67</v>
-      </c>
-      <c r="L24" t="s">
-        <v>66</v>
-      </c>
-      <c r="M24" t="s">
-        <v>67</v>
-      </c>
-      <c r="N24" t="s">
-        <v>68</v>
-      </c>
-      <c r="O24" t="s">
-        <v>69</v>
-      </c>
-      <c r="P24" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>71</v>
-      </c>
-      <c r="R24" t="s">
-        <v>72</v>
-      </c>
-      <c r="S24" t="s">
-        <v>73</v>
-      </c>
-      <c r="T24" t="s">
-        <v>74</v>
-      </c>
-      <c r="U24" t="s">
-        <v>75</v>
-      </c>
-      <c r="V24" t="s">
-        <v>68</v>
-      </c>
-      <c r="W24" t="s">
-        <v>69</v>
-      </c>
-      <c r="X24" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB24" t="s">
-        <v>125</v>
-      </c>
-      <c r="AC24" s="3">
-        <v>2.2080000000000002</v>
-      </c>
-      <c r="AD24" s="3">
-        <v>1.6180000000000001</v>
-      </c>
-      <c r="AE24" s="5">
-        <v>7.4000000000000004</v>
-      </c>
-      <c r="AF24" s="5">
-        <v>13.1</v>
-      </c>
-      <c r="AG24">
-        <v>333</v>
-      </c>
-      <c r="AH24" s="5">
-        <v>6.7999999999999998</v>
-      </c>
-      <c r="AI24" s="5">
-        <v>17.800000000000001</v>
-      </c>
-      <c r="AJ24" s="5">
-        <v>8.5</v>
-      </c>
-      <c r="AK24" s="4">
-        <v>5.2199999999999998</v>
-      </c>
-      <c r="AL24" s="4">
-        <v>0.14999999999999999</v>
-      </c>
-      <c r="AM24" s="3">
-        <v>16.972000000000001</v>
-      </c>
-      <c r="AN24" s="5">
-        <v>26.600000000000001</v>
-      </c>
-      <c r="AO24" s="5">
-        <v>90.700000000000003</v>
-      </c>
-      <c r="AP24" s="4">
-        <v>0.01</v>
-      </c>
-      <c r="AQ24" s="3">
-        <v>4.7830000000000004</v>
-      </c>
-      <c r="AR24" s="3">
-        <v>0.039</v>
-      </c>
-      <c r="AS24" s="5">
-        <v>7.2999999999999998</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>126</v>
-      </c>
-      <c r="B25" t="s">
-        <v>82</v>
-      </c>
-      <c r="C25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" s="2">
-        <v>35.062860999999998</v>
-      </c>
-      <c r="F25" s="2">
-        <v>126.772972</v>
-      </c>
-      <c r="G25" t="s">
-        <v>66</v>
-      </c>
-      <c r="H25" t="s">
-        <v>67</v>
-      </c>
-      <c r="L25" t="s">
-        <v>66</v>
-      </c>
-      <c r="M25" t="s">
-        <v>67</v>
-      </c>
-      <c r="N25" t="s">
-        <v>68</v>
-      </c>
-      <c r="O25" t="s">
-        <v>69</v>
-      </c>
-      <c r="P25" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>71</v>
-      </c>
-      <c r="R25" t="s">
-        <v>72</v>
-      </c>
-      <c r="S25" t="s">
-        <v>73</v>
-      </c>
-      <c r="T25" t="s">
-        <v>74</v>
-      </c>
-      <c r="U25" t="s">
-        <v>75</v>
-      </c>
-      <c r="V25" t="s">
-        <v>68</v>
-      </c>
-      <c r="W25" t="s">
-        <v>69</v>
-      </c>
-      <c r="X25" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA25" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB25" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC25" s="4">
-        <v>0.92000000000000004</v>
-      </c>
-      <c r="AD25" s="4">
-        <v>1.49</v>
-      </c>
-      <c r="AE25" s="5">
-        <v>7.2000000000000002</v>
-      </c>
-      <c r="AF25" s="5">
-        <v>10.800000000000001</v>
-      </c>
-      <c r="AG25">
-        <v>184</v>
-      </c>
-      <c r="AH25" s="5">
-        <v>6.9000000000000004</v>
-      </c>
-      <c r="AI25" s="5">
-        <v>24.199999999999999</v>
-      </c>
-      <c r="AJ25" s="5">
-        <v>5.4000000000000004</v>
-      </c>
-      <c r="AK25" s="3">
-        <v>3.173</v>
-      </c>
-      <c r="AL25" s="3">
-        <v>0.19600000000000001</v>
-      </c>
-      <c r="AM25" s="4">
-        <v>57.43</v>
-      </c>
-      <c r="AN25" s="5">
-        <v>24.600000000000001</v>
-      </c>
-      <c r="AO25" s="5">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="AP25" s="3">
-        <v>0.129</v>
-      </c>
-      <c r="AQ25" s="3">
-        <v>3.1040000000000001</v>
-      </c>
-      <c r="AR25" s="3">
-        <v>0.153</v>
-      </c>
-      <c r="AS25" s="5">
-        <v>7.0999999999999996</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>128</v>
-      </c>
-      <c r="B26" t="s">
-        <v>85</v>
-      </c>
-      <c r="C26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" t="s">
-        <v>65</v>
-      </c>
-      <c r="E26" s="2">
-        <v>35.062860999999998</v>
-      </c>
-      <c r="F26" s="2">
-        <v>126.772972</v>
-      </c>
-      <c r="G26" t="s">
-        <v>66</v>
-      </c>
-      <c r="H26" t="s">
-        <v>67</v>
-      </c>
-      <c r="L26" t="s">
-        <v>66</v>
-      </c>
-      <c r="M26" t="s">
-        <v>67</v>
-      </c>
-      <c r="N26" t="s">
-        <v>68</v>
-      </c>
-      <c r="O26" t="s">
-        <v>69</v>
-      </c>
-      <c r="P26" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>71</v>
-      </c>
-      <c r="R26" t="s">
-        <v>72</v>
-      </c>
-      <c r="S26" t="s">
-        <v>73</v>
-      </c>
-      <c r="T26" t="s">
-        <v>74</v>
-      </c>
-      <c r="U26" t="s">
-        <v>75</v>
-      </c>
-      <c r="V26" t="s">
-        <v>68</v>
-      </c>
-      <c r="W26" t="s">
-        <v>69</v>
-      </c>
-      <c r="X26" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z26" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA26" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB26" t="s">
-        <v>129</v>
-      </c>
-      <c r="AC26" s="3">
-        <v>0.70799999999999996</v>
-      </c>
-      <c r="AD26" s="3">
-        <v>1.982</v>
-      </c>
-      <c r="AE26" s="5">
-        <v>7.2999999999999998</v>
-      </c>
-      <c r="AF26" s="5">
-        <v>10.1</v>
-      </c>
-      <c r="AG26">
-        <v>243</v>
-      </c>
-      <c r="AH26" s="5">
-        <v>5.5999999999999996</v>
-      </c>
-      <c r="AI26" s="5">
-        <v>12.199999999999999</v>
-      </c>
-      <c r="AJ26" s="5">
-        <v>7.2999999999999998</v>
-      </c>
-      <c r="AK26" s="3">
-        <v>3.6829999999999998</v>
-      </c>
-      <c r="AL26" s="3">
-        <v>0.128</v>
-      </c>
-      <c r="AM26" s="5">
-        <v>31.5</v>
-      </c>
-      <c r="AN26" s="5">
-        <v>26.100000000000001</v>
-      </c>
-      <c r="AO26" s="5">
-        <v>57.399999999999999</v>
-      </c>
-      <c r="AP26" s="3">
-        <v>0.023</v>
-      </c>
-      <c r="AQ26" s="3">
-        <v>3.4249999999999998</v>
-      </c>
-      <c r="AR26" s="3">
-        <v>0.045999999999999999</v>
-      </c>
-      <c r="AS26" s="5">
-        <v>6.2999999999999998</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>130</v>
-      </c>
-      <c r="B27" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" t="s">
-        <v>64</v>
-      </c>
-      <c r="D27" t="s">
-        <v>65</v>
-      </c>
-      <c r="E27" s="2">
-        <v>35.062860999999998</v>
-      </c>
-      <c r="F27" s="2">
-        <v>126.772972</v>
-      </c>
-      <c r="G27" t="s">
-        <v>66</v>
-      </c>
-      <c r="H27" t="s">
-        <v>67</v>
-      </c>
-      <c r="L27" t="s">
-        <v>66</v>
-      </c>
-      <c r="M27" t="s">
-        <v>67</v>
-      </c>
-      <c r="N27" t="s">
-        <v>68</v>
-      </c>
-      <c r="O27" t="s">
-        <v>69</v>
-      </c>
-      <c r="P27" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>71</v>
-      </c>
-      <c r="R27" t="s">
-        <v>72</v>
-      </c>
-      <c r="S27" t="s">
-        <v>73</v>
-      </c>
-      <c r="T27" t="s">
-        <v>74</v>
-      </c>
-      <c r="U27" t="s">
-        <v>75</v>
-      </c>
-      <c r="V27" t="s">
-        <v>68</v>
-      </c>
-      <c r="W27" t="s">
-        <v>69</v>
-      </c>
-      <c r="X27" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z27" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA27" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB27" t="s">
-        <v>131</v>
-      </c>
-      <c r="AC27" s="3">
-        <v>1.0249999999999999</v>
-      </c>
-      <c r="AD27" s="3">
-        <v>1.413</v>
-      </c>
-      <c r="AE27" s="5">
-        <v>7.5</v>
-      </c>
-      <c r="AF27" s="5">
-        <v>9.9000000000000004</v>
-      </c>
-      <c r="AG27">
-        <v>228</v>
-      </c>
-      <c r="AH27">
-        <v>6</v>
-      </c>
-      <c r="AI27" s="5">
-        <v>11.1</v>
-      </c>
-      <c r="AJ27" s="5">
-        <v>5.5</v>
-      </c>
-      <c r="AK27" s="3">
-        <v>3.282</v>
-      </c>
-      <c r="AL27" s="3">
-        <v>0.19800000000000001</v>
-      </c>
-      <c r="AM27" s="3">
-        <v>29.734999999999999</v>
-      </c>
-      <c r="AN27" s="5">
-        <v>23.100000000000001</v>
-      </c>
-      <c r="AO27" s="5">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="AP27" s="3">
-        <v>0.11899999999999999</v>
-      </c>
-      <c r="AQ27" s="3">
-        <v>3.1949999999999998</v>
-      </c>
-      <c r="AR27" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="AS27" s="5">
-        <v>7.5999999999999996</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>132</v>
-      </c>
-      <c r="B28" t="s">
-        <v>79</v>
-      </c>
-      <c r="C28" t="s">
-        <v>64</v>
-      </c>
-      <c r="D28" t="s">
-        <v>65</v>
-      </c>
-      <c r="E28" s="2">
-        <v>35.062860999999998</v>
-      </c>
-      <c r="F28" s="2">
-        <v>126.772972</v>
-      </c>
-      <c r="G28" t="s">
-        <v>66</v>
-      </c>
-      <c r="H28" t="s">
-        <v>67</v>
-      </c>
-      <c r="L28" t="s">
-        <v>66</v>
-      </c>
-      <c r="M28" t="s">
-        <v>67</v>
-      </c>
-      <c r="N28" t="s">
-        <v>68</v>
-      </c>
-      <c r="O28" t="s">
-        <v>69</v>
-      </c>
-      <c r="P28" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>71</v>
-      </c>
-      <c r="R28" t="s">
-        <v>72</v>
-      </c>
-      <c r="S28" t="s">
-        <v>73</v>
-      </c>
-      <c r="T28" t="s">
-        <v>74</v>
-      </c>
-      <c r="U28" t="s">
-        <v>75</v>
-      </c>
-      <c r="V28" t="s">
-        <v>68</v>
-      </c>
-      <c r="W28" t="s">
-        <v>69</v>
-      </c>
-      <c r="X28" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y28" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z28" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA28" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB28" t="s">
-        <v>133</v>
-      </c>
-      <c r="AC28" s="3">
-        <v>1.411</v>
-      </c>
-      <c r="AD28" s="3">
-        <v>1.7949999999999999</v>
-      </c>
-      <c r="AE28" s="5">
-        <v>6.9000000000000004</v>
-      </c>
-      <c r="AF28" s="5">
-        <v>8.4000000000000004</v>
-      </c>
-      <c r="AG28">
-        <v>274</v>
-      </c>
-      <c r="AH28" s="5">
-        <v>5.5</v>
-      </c>
-      <c r="AI28" s="5">
-        <v>10.5</v>
-      </c>
-      <c r="AJ28" s="5">
-        <v>6.5999999999999996</v>
-      </c>
-      <c r="AK28" s="3">
-        <v>4.0650000000000004</v>
-      </c>
-      <c r="AL28" s="4">
-        <v>0.11</v>
-      </c>
-      <c r="AM28" s="3">
-        <v>20.491</v>
-      </c>
-      <c r="AN28" s="5">
-        <v>23.800000000000001</v>
-      </c>
-      <c r="AO28" s="5">
-        <v>25.699999999999999</v>
-      </c>
-      <c r="AP28" s="3">
-        <v>0.055</v>
-      </c>
-      <c r="AQ28" s="3">
-        <v>3.9140000000000001</v>
-      </c>
-      <c r="AR28" s="4">
-        <v>0.070000000000000007</v>
-      </c>
-      <c r="AS28" s="5">
-        <v>6.2000000000000002</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>134</v>
-      </c>
-      <c r="B29" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" t="s">
-        <v>64</v>
-      </c>
-      <c r="D29" t="s">
-        <v>65</v>
-      </c>
-      <c r="E29" s="2">
-        <v>35.062860999999998</v>
-      </c>
-      <c r="F29" s="2">
-        <v>126.772972</v>
-      </c>
-      <c r="G29" t="s">
-        <v>66</v>
-      </c>
-      <c r="H29" t="s">
-        <v>67</v>
-      </c>
-      <c r="L29" t="s">
-        <v>66</v>
-      </c>
-      <c r="M29" t="s">
-        <v>67</v>
-      </c>
-      <c r="N29" t="s">
-        <v>68</v>
-      </c>
-      <c r="O29" t="s">
-        <v>69</v>
-      </c>
-      <c r="P29" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>71</v>
-      </c>
-      <c r="R29" t="s">
-        <v>72</v>
-      </c>
-      <c r="S29" t="s">
-        <v>73</v>
-      </c>
-      <c r="T29" t="s">
-        <v>74</v>
-      </c>
-      <c r="U29" t="s">
-        <v>75</v>
-      </c>
-      <c r="V29" t="s">
-        <v>68</v>
-      </c>
-      <c r="W29" t="s">
-        <v>69</v>
-      </c>
-      <c r="X29" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y29" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z29" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA29" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB29" t="s">
-        <v>135</v>
-      </c>
-      <c r="AC29" s="4">
-        <v>0.52000000000000002</v>
-      </c>
-      <c r="AD29" s="3">
-        <v>1.871</v>
-      </c>
-      <c r="AE29" s="5">
-        <v>7.4000000000000004</v>
-      </c>
-      <c r="AF29" s="5">
-        <v>6.9000000000000004</v>
-      </c>
-      <c r="AG29">
-        <v>146</v>
-      </c>
-      <c r="AH29" s="5">
-        <v>3.6000000000000001</v>
-      </c>
-      <c r="AI29" s="5">
-        <v>25.699999999999999</v>
-      </c>
-      <c r="AJ29" s="5">
-        <v>7.4000000000000004</v>
-      </c>
-      <c r="AK29" s="3">
-        <v>2.9980000000000002</v>
-      </c>
-      <c r="AL29" s="4">
-        <v>0.17000000000000001</v>
-      </c>
-      <c r="AM29" s="3">
-        <v>166.56200000000001</v>
-      </c>
-      <c r="AN29" s="5">
-        <v>20.600000000000001</v>
-      </c>
-      <c r="AO29" s="5">
-        <v>5.7000000000000002</v>
-      </c>
-      <c r="AP29" s="3">
-        <v>0.11600000000000001</v>
-      </c>
-      <c r="AQ29" s="3">
-        <v>2.7519999999999998</v>
-      </c>
-      <c r="AR29" s="3">
-        <v>0.127</v>
-      </c>
-      <c r="AS29">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>136</v>
-      </c>
-      <c r="B30" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" t="s">
-        <v>64</v>
-      </c>
-      <c r="D30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" s="2">
-        <v>35.062860999999998</v>
-      </c>
-      <c r="F30" s="2">
-        <v>126.772972</v>
-      </c>
-      <c r="G30" t="s">
-        <v>66</v>
-      </c>
-      <c r="H30" t="s">
-        <v>67</v>
-      </c>
-      <c r="L30" t="s">
-        <v>66</v>
-      </c>
-      <c r="M30" t="s">
-        <v>67</v>
-      </c>
-      <c r="N30" t="s">
-        <v>68</v>
-      </c>
-      <c r="O30" t="s">
-        <v>69</v>
-      </c>
-      <c r="P30" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>71</v>
-      </c>
-      <c r="R30" t="s">
-        <v>72</v>
-      </c>
-      <c r="S30" t="s">
-        <v>73</v>
-      </c>
-      <c r="T30" t="s">
-        <v>74</v>
-      </c>
-      <c r="U30" t="s">
-        <v>75</v>
-      </c>
-      <c r="V30" t="s">
-        <v>68</v>
-      </c>
-      <c r="W30" t="s">
-        <v>69</v>
-      </c>
-      <c r="X30" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y30" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z30" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA30" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB30" t="s">
-        <v>137</v>
-      </c>
-      <c r="AC30" s="3">
-        <v>1.1319999999999999</v>
-      </c>
-      <c r="AD30" s="3">
-        <v>1.796</v>
-      </c>
-      <c r="AE30" s="5">
-        <v>6.9000000000000004</v>
-      </c>
-      <c r="AF30" s="5">
-        <v>6.2999999999999998</v>
-      </c>
-      <c r="AG30">
-        <v>225</v>
-      </c>
-      <c r="AH30" s="5">
-        <v>3.5</v>
-      </c>
-      <c r="AI30">
-        <v>11</v>
-      </c>
-      <c r="AJ30" s="5">
-        <v>7.4000000000000004</v>
-      </c>
-      <c r="AK30" s="3">
-        <v>3.496</v>
-      </c>
-      <c r="AL30" s="3">
-        <v>0.126</v>
-      </c>
-      <c r="AM30" s="3">
-        <v>57.512999999999998</v>
-      </c>
-      <c r="AN30" s="5">
-        <v>25.100000000000001</v>
-      </c>
-      <c r="AO30" s="5">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="AP30" s="3">
-        <v>0.083000000000000004</v>
-      </c>
-      <c r="AQ30" s="3">
-        <v>3.3860000000000001</v>
-      </c>
-      <c r="AR30" s="3">
-        <v>0.096000000000000002</v>
-      </c>
-      <c r="AS30" s="5">
-        <v>4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>138</v>
-      </c>
-      <c r="B31" t="s">
-        <v>104</v>
-      </c>
-      <c r="C31" t="s">
-        <v>64</v>
-      </c>
-      <c r="D31" t="s">
-        <v>65</v>
-      </c>
-      <c r="E31" s="2">
-        <v>35.062860999999998</v>
-      </c>
-      <c r="F31" s="2">
-        <v>126.772972</v>
-      </c>
-      <c r="G31" t="s">
-        <v>66</v>
-      </c>
-      <c r="H31" t="s">
-        <v>67</v>
-      </c>
-      <c r="L31" t="s">
-        <v>66</v>
-      </c>
-      <c r="M31" t="s">
-        <v>67</v>
-      </c>
-      <c r="N31" t="s">
-        <v>68</v>
-      </c>
-      <c r="O31" t="s">
-        <v>69</v>
-      </c>
-      <c r="P31" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>71</v>
-      </c>
-      <c r="R31" t="s">
-        <v>72</v>
-      </c>
-      <c r="S31" t="s">
-        <v>73</v>
-      </c>
-      <c r="T31" t="s">
-        <v>74</v>
-      </c>
-      <c r="U31" t="s">
-        <v>75</v>
-      </c>
-      <c r="V31" t="s">
-        <v>68</v>
-      </c>
-      <c r="W31" t="s">
-        <v>69</v>
-      </c>
-      <c r="X31" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y31" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA31" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB31" t="s">
-        <v>139</v>
-      </c>
-      <c r="AC31" s="3">
-        <v>0.61199999999999999</v>
-      </c>
-      <c r="AD31" s="3">
-        <v>1.7390000000000001</v>
-      </c>
-      <c r="AE31">
-        <v>7</v>
-      </c>
-      <c r="AF31" s="5">
-        <v>5.9000000000000004</v>
-      </c>
-      <c r="AG31">
-        <v>162</v>
-      </c>
-      <c r="AH31" s="5">
-        <v>3.1000000000000001</v>
-      </c>
-      <c r="AI31">
-        <v>8</v>
-      </c>
-      <c r="AJ31" s="5">
-        <v>7.4000000000000004</v>
-      </c>
-      <c r="AK31" s="3">
-        <v>2.7690000000000001</v>
-      </c>
-      <c r="AL31" s="4">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="AM31" s="3">
-        <v>93.861999999999995</v>
-      </c>
-      <c r="AN31" s="5">
-        <v>23.100000000000001</v>
-      </c>
-      <c r="AO31">
-        <v>6</v>
-      </c>
-      <c r="AP31" s="5">
-        <v>0.10000000000000001</v>
-      </c>
-      <c r="AQ31" s="3">
-        <v>2.738</v>
-      </c>
-      <c r="AR31" s="3">
-        <v>0.114</v>
-      </c>
-      <c r="AS31" s="5">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>140</v>
-      </c>
-      <c r="B32" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32" t="s">
-        <v>65</v>
-      </c>
-      <c r="E32" s="2">
-        <v>35.062860999999998</v>
-      </c>
-      <c r="F32" s="2">
-        <v>126.772972</v>
-      </c>
-      <c r="G32" t="s">
-        <v>66</v>
-      </c>
-      <c r="H32" t="s">
-        <v>67</v>
-      </c>
-      <c r="L32" t="s">
-        <v>66</v>
-      </c>
-      <c r="M32" t="s">
-        <v>67</v>
-      </c>
-      <c r="N32" t="s">
-        <v>68</v>
-      </c>
-      <c r="O32" t="s">
-        <v>69</v>
-      </c>
-      <c r="P32" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>71</v>
-      </c>
-      <c r="R32" t="s">
-        <v>72</v>
-      </c>
-      <c r="S32" t="s">
-        <v>73</v>
-      </c>
-      <c r="T32" t="s">
-        <v>74</v>
-      </c>
-      <c r="U32" t="s">
-        <v>75</v>
-      </c>
-      <c r="V32" t="s">
-        <v>68</v>
-      </c>
-      <c r="W32" t="s">
-        <v>69</v>
-      </c>
-      <c r="X32" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y32" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z32" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA32" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB32" t="s">
-        <v>141</v>
-      </c>
-      <c r="AC32" s="3">
-        <v>0.75900000000000001</v>
-      </c>
-      <c r="AD32" s="4">
-        <v>1.8799999999999999</v>
-      </c>
-      <c r="AE32" s="5">
-        <v>7.5999999999999996</v>
-      </c>
-      <c r="AF32" s="5">
-        <v>5.7000000000000002</v>
-      </c>
-      <c r="AG32">
-        <v>182</v>
-      </c>
-      <c r="AH32" s="5">
-        <v>3.8999999999999999</v>
-      </c>
-      <c r="AI32" s="5">
-        <v>13.699999999999999</v>
-      </c>
-      <c r="AJ32" s="5">
-        <v>6.5</v>
-      </c>
-      <c r="AK32" s="3">
-        <v>3.169</v>
-      </c>
-      <c r="AL32" s="3">
-        <v>0.154</v>
-      </c>
-      <c r="AM32" s="3">
-        <v>73.293999999999997</v>
-      </c>
-      <c r="AN32" s="5">
-        <v>25.300000000000001</v>
-      </c>
-      <c r="AO32" s="5">
-        <v>5.2000000000000002</v>
-      </c>
-      <c r="AP32" s="3">
-        <v>0.13100000000000001</v>
-      </c>
-      <c r="AQ32" s="3">
-        <v>3.1520000000000001</v>
-      </c>
-      <c r="AR32" s="3">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="AS32" s="5">
-        <v>4.2000000000000002</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>142</v>
-      </c>
-      <c r="B33" t="s">
-        <v>79</v>
-      </c>
-      <c r="C33" t="s">
-        <v>64</v>
-      </c>
-      <c r="D33" t="s">
-        <v>65</v>
-      </c>
-      <c r="E33" s="2">
-        <v>35.062860999999998</v>
-      </c>
-      <c r="F33" s="2">
-        <v>126.772972</v>
-      </c>
-      <c r="G33" t="s">
-        <v>66</v>
-      </c>
-      <c r="H33" t="s">
-        <v>67</v>
-      </c>
-      <c r="L33" t="s">
-        <v>66</v>
-      </c>
-      <c r="M33" t="s">
-        <v>67</v>
-      </c>
-      <c r="N33" t="s">
-        <v>68</v>
-      </c>
-      <c r="O33" t="s">
-        <v>69</v>
-      </c>
-      <c r="P33" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>71</v>
-      </c>
-      <c r="R33" t="s">
-        <v>72</v>
-      </c>
-      <c r="S33" t="s">
-        <v>73</v>
-      </c>
-      <c r="T33" t="s">
-        <v>74</v>
-      </c>
-      <c r="U33" t="s">
-        <v>75</v>
-      </c>
-      <c r="V33" t="s">
-        <v>68</v>
-      </c>
-      <c r="W33" t="s">
-        <v>69</v>
-      </c>
-      <c r="X33" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y33" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z33" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA33" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB33" t="s">
-        <v>143</v>
-      </c>
-      <c r="AC33" s="3">
-        <v>1.073</v>
-      </c>
-      <c r="AD33" s="3">
-        <v>1.736</v>
-      </c>
-      <c r="AE33" s="5">
-        <v>7.5999999999999996</v>
-      </c>
-      <c r="AF33" s="5">
-        <v>7.7999999999999998</v>
-      </c>
-      <c r="AG33">
-        <v>244</v>
-      </c>
-      <c r="AH33" s="5">
-        <v>4.2999999999999998</v>
-      </c>
-      <c r="AI33" s="5">
-        <v>5.7000000000000002</v>
-      </c>
-      <c r="AJ33" s="5">
-        <v>7.9000000000000004</v>
-      </c>
-      <c r="AK33" s="3">
-        <v>3.472</v>
-      </c>
-      <c r="AL33" s="4">
-        <v>0.17999999999999999</v>
-      </c>
-      <c r="AM33" s="3">
-        <v>35.363</v>
-      </c>
-      <c r="AN33" s="5">
-        <v>29.699999999999999</v>
-      </c>
-      <c r="AO33" s="5">
-        <v>57.5</v>
-      </c>
-      <c r="AP33" s="3">
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="AQ33" s="4">
-        <v>3.3599999999999999</v>
-      </c>
-      <c r="AR33" s="3">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="AS33" s="5">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>144</v>
-      </c>
-      <c r="B34" t="s">
-        <v>82</v>
-      </c>
-      <c r="C34" t="s">
-        <v>64</v>
-      </c>
-      <c r="D34" t="s">
-        <v>65</v>
-      </c>
-      <c r="E34" s="2">
-        <v>35.062860999999998</v>
-      </c>
-      <c r="F34" s="2">
-        <v>126.772972</v>
-      </c>
-      <c r="G34" t="s">
-        <v>66</v>
-      </c>
-      <c r="H34" t="s">
-        <v>67</v>
-      </c>
-      <c r="L34" t="s">
-        <v>66</v>
-      </c>
-      <c r="M34" t="s">
-        <v>67</v>
-      </c>
-      <c r="N34" t="s">
-        <v>68</v>
-      </c>
-      <c r="O34" t="s">
-        <v>69</v>
-      </c>
-      <c r="P34" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>71</v>
-      </c>
-      <c r="R34" t="s">
-        <v>72</v>
-      </c>
-      <c r="S34" t="s">
-        <v>73</v>
-      </c>
-      <c r="T34" t="s">
-        <v>74</v>
-      </c>
-      <c r="U34" t="s">
-        <v>75</v>
-      </c>
-      <c r="V34" t="s">
-        <v>68</v>
-      </c>
-      <c r="W34" t="s">
-        <v>69</v>
-      </c>
-      <c r="X34" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y34" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z34" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA34" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB34" t="s">
-        <v>145</v>
-      </c>
-      <c r="AC34" s="3">
-        <v>1.6579999999999999</v>
-      </c>
-      <c r="AD34" s="3">
-        <v>1.4570000000000001</v>
-      </c>
-      <c r="AE34">
-        <v>7</v>
-      </c>
-      <c r="AF34" s="5">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="AG34">
-        <v>284</v>
-      </c>
-      <c r="AH34" s="5">
-        <v>4.7000000000000002</v>
-      </c>
-      <c r="AI34" s="5">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="AJ34">
-        <v>7</v>
-      </c>
-      <c r="AK34" s="4">
-        <v>4.2400000000000002</v>
-      </c>
-      <c r="AL34" s="4">
-        <v>0.11</v>
-      </c>
-      <c r="AM34" s="3">
-        <v>26.385000000000002</v>
-      </c>
-      <c r="AN34" s="5">
-        <v>29.300000000000001</v>
-      </c>
-      <c r="AO34" s="5">
-        <v>45.299999999999997</v>
-      </c>
-      <c r="AP34" s="3">
-        <v>0.037999999999999999</v>
-      </c>
-      <c r="AQ34" s="4">
-        <v>3.9900000000000002</v>
-      </c>
-      <c r="AR34" s="3">
-        <v>0.065000000000000002</v>
-      </c>
-      <c r="AS34">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>146</v>
-      </c>
-      <c r="B35" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" t="s">
-        <v>64</v>
-      </c>
-      <c r="D35" t="s">
-        <v>65</v>
-      </c>
-      <c r="E35" s="2">
-        <v>35.062860999999998</v>
-      </c>
-      <c r="F35" s="2">
-        <v>126.772972</v>
-      </c>
-      <c r="G35" t="s">
-        <v>66</v>
-      </c>
-      <c r="H35" t="s">
-        <v>67</v>
-      </c>
-      <c r="L35" t="s">
-        <v>66</v>
-      </c>
-      <c r="M35" t="s">
-        <v>67</v>
-      </c>
-      <c r="N35" t="s">
-        <v>68</v>
-      </c>
-      <c r="O35" t="s">
-        <v>69</v>
-      </c>
-      <c r="P35" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>71</v>
-      </c>
-      <c r="R35" t="s">
-        <v>72</v>
-      </c>
-      <c r="S35" t="s">
-        <v>73</v>
-      </c>
-      <c r="T35" t="s">
-        <v>74</v>
-      </c>
-      <c r="U35" t="s">
-        <v>75</v>
-      </c>
-      <c r="V35" t="s">
-        <v>68</v>
-      </c>
-      <c r="W35" t="s">
-        <v>69</v>
-      </c>
-      <c r="X35" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y35" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z35" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA35" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB35" t="s">
-        <v>147</v>
-      </c>
-      <c r="AC35" s="4">
-        <v>0.54000000000000004</v>
-      </c>
-      <c r="AD35" s="3">
-        <v>1.3160000000000001</v>
-      </c>
-      <c r="AE35" s="5">
-        <v>6.7000000000000002</v>
-      </c>
-      <c r="AF35">
-        <v>8</v>
-      </c>
-      <c r="AG35">
-        <v>165</v>
-      </c>
-      <c r="AH35" s="5">
-        <v>4.7999999999999998</v>
-      </c>
-      <c r="AI35" s="5">
-        <v>50.200000000000003</v>
-      </c>
-      <c r="AJ35" s="5">
-        <v>6.0999999999999996</v>
-      </c>
-      <c r="AK35" s="3">
-        <v>2.5110000000000001</v>
-      </c>
-      <c r="AL35" s="3">
-        <v>0.218</v>
-      </c>
-      <c r="AM35" s="3">
-        <v>101.789</v>
-      </c>
-      <c r="AN35" s="5">
-        <v>28.300000000000001</v>
-      </c>
-      <c r="AO35" s="5">
-        <v>24.100000000000001</v>
-      </c>
-      <c r="AP35" s="3">
-        <v>0.10100000000000001</v>
-      </c>
-      <c r="AQ35" s="3">
-        <v>2.282</v>
-      </c>
-      <c r="AR35" s="3">
-        <v>0.121</v>
-      </c>
-      <c r="AS35" s="5">
-        <v>5.2000000000000002</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>148</v>
-      </c>
-      <c r="B36" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" t="s">
-        <v>64</v>
-      </c>
-      <c r="D36" t="s">
-        <v>65</v>
-      </c>
-      <c r="E36" s="2">
-        <v>35.062860999999998</v>
-      </c>
-      <c r="F36" s="2">
-        <v>126.772972</v>
-      </c>
-      <c r="G36" t="s">
-        <v>66</v>
-      </c>
-      <c r="H36" t="s">
-        <v>67</v>
-      </c>
-      <c r="L36" t="s">
-        <v>66</v>
-      </c>
-      <c r="M36" t="s">
-        <v>67</v>
-      </c>
-      <c r="N36" t="s">
-        <v>68</v>
-      </c>
-      <c r="O36" t="s">
-        <v>69</v>
-      </c>
-      <c r="P36" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>71</v>
-      </c>
-      <c r="R36" t="s">
-        <v>72</v>
-      </c>
-      <c r="S36" t="s">
-        <v>73</v>
-      </c>
-      <c r="T36" t="s">
-        <v>74</v>
-      </c>
-      <c r="U36" t="s">
-        <v>75</v>
-      </c>
-      <c r="V36" t="s">
-        <v>68</v>
-      </c>
-      <c r="W36" t="s">
-        <v>69</v>
-      </c>
-      <c r="X36" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y36" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z36" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA36" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB36" t="s">
-        <v>149</v>
-      </c>
-      <c r="AC36" s="3">
-        <v>0.378</v>
-      </c>
-      <c r="AD36" s="3">
-        <v>1.3129999999999999</v>
-      </c>
-      <c r="AE36" s="5">
-        <v>7.0999999999999996</v>
-      </c>
-      <c r="AF36" s="5">
-        <v>6.4000000000000004</v>
-      </c>
-      <c r="AG36">
-        <v>140</v>
-      </c>
-      <c r="AH36" s="5">
-        <v>3.7000000000000002</v>
-      </c>
-      <c r="AI36" s="5">
-        <v>28.699999999999999</v>
-      </c>
-      <c r="AJ36" s="5">
-        <v>7.4000000000000004</v>
-      </c>
-      <c r="AK36" s="3">
-        <v>2.218</v>
-      </c>
-      <c r="AL36" s="3">
-        <v>0.17199999999999999</v>
-      </c>
-      <c r="AM36" s="3">
-        <v>139.75299999999999</v>
-      </c>
-      <c r="AN36" s="5">
-        <v>21.5</v>
-      </c>
-      <c r="AO36" s="5">
-        <v>4.2000000000000002</v>
-      </c>
-      <c r="AP36" s="4">
-        <v>0.11</v>
-      </c>
-      <c r="AQ36" s="4">
-        <v>2.1400000000000001</v>
-      </c>
-      <c r="AR36" s="3">
-        <v>0.124</v>
-      </c>
-      <c r="AS36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s">
-        <v>150</v>
-      </c>
-      <c r="B37" t="s">
-        <v>82</v>
-      </c>
-      <c r="C37" t="s">
-        <v>64</v>
-      </c>
-      <c r="D37" t="s">
-        <v>65</v>
-      </c>
-      <c r="E37" s="2">
-        <v>35.062860999999998</v>
-      </c>
-      <c r="F37" s="2">
-        <v>126.772972</v>
-      </c>
-      <c r="G37" t="s">
-        <v>66</v>
-      </c>
-      <c r="H37" t="s">
-        <v>67</v>
-      </c>
-      <c r="L37" t="s">
-        <v>66</v>
-      </c>
-      <c r="M37" t="s">
-        <v>67</v>
-      </c>
-      <c r="N37" t="s">
-        <v>68</v>
-      </c>
-      <c r="O37" t="s">
-        <v>69</v>
-      </c>
-      <c r="P37" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>71</v>
-      </c>
-      <c r="R37" t="s">
-        <v>72</v>
-      </c>
-      <c r="S37" t="s">
-        <v>73</v>
-      </c>
-      <c r="T37" t="s">
-        <v>74</v>
-      </c>
-      <c r="U37" t="s">
-        <v>75</v>
-      </c>
-      <c r="V37" t="s">
-        <v>68</v>
-      </c>
-      <c r="W37" t="s">
-        <v>69</v>
-      </c>
-      <c r="X37" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y37" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z37" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA37" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB37" t="s">
-        <v>151</v>
-      </c>
-      <c r="AC37" s="3">
-        <v>0.48899999999999999</v>
-      </c>
-      <c r="AD37" s="3">
-        <v>1.613</v>
-      </c>
-      <c r="AE37" s="5">
-        <v>7.0999999999999996</v>
-      </c>
-      <c r="AF37" s="5">
-        <v>5.4000000000000004</v>
-      </c>
-      <c r="AG37">
-        <v>172</v>
-      </c>
-      <c r="AH37" s="5">
-        <v>3.1000000000000001</v>
-      </c>
-      <c r="AI37" s="5">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="AJ37" s="5">
-        <v>7.2000000000000002</v>
-      </c>
-      <c r="AK37" s="3">
-        <v>2.5449999999999999</v>
-      </c>
-      <c r="AL37" s="3">
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="AM37" s="4">
-        <v>81.349999999999994</v>
-      </c>
-      <c r="AN37" s="5">
-        <v>23.300000000000001</v>
-      </c>
-      <c r="AO37">
-        <v>6</v>
-      </c>
-      <c r="AP37" s="5">
-        <v>0.10000000000000001</v>
-      </c>
-      <c r="AQ37" s="3">
-        <v>2.5009999999999999</v>
-      </c>
-      <c r="AR37" s="3">
-        <v>0.111</v>
-      </c>
-      <c r="AS37" s="5">
-        <v>3.2999999999999998</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s">
-        <v>152</v>
-      </c>
-      <c r="B38" t="s">
-        <v>85</v>
-      </c>
-      <c r="C38" t="s">
-        <v>64</v>
-      </c>
-      <c r="D38" t="s">
-        <v>65</v>
-      </c>
-      <c r="E38" s="2">
-        <v>35.062860999999998</v>
-      </c>
-      <c r="F38" s="2">
-        <v>126.772972</v>
-      </c>
-      <c r="G38" t="s">
-        <v>66</v>
-      </c>
-      <c r="H38" t="s">
-        <v>67</v>
-      </c>
-      <c r="L38" t="s">
-        <v>66</v>
-      </c>
-      <c r="M38" t="s">
-        <v>67</v>
-      </c>
-      <c r="N38" t="s">
-        <v>68</v>
-      </c>
-      <c r="O38" t="s">
-        <v>69</v>
-      </c>
-      <c r="P38" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>71</v>
-      </c>
-      <c r="R38" t="s">
-        <v>72</v>
-      </c>
-      <c r="S38" t="s">
-        <v>73</v>
-      </c>
-      <c r="T38" t="s">
-        <v>74</v>
-      </c>
-      <c r="U38" t="s">
-        <v>75</v>
-      </c>
-      <c r="V38" t="s">
-        <v>68</v>
-      </c>
-      <c r="W38" t="s">
-        <v>69</v>
-      </c>
-      <c r="X38" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y38" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z38" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA38" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB38" t="s">
-        <v>153</v>
-      </c>
-      <c r="AC38" s="3">
-        <v>0.36499999999999999</v>
-      </c>
-      <c r="AD38" s="3">
-        <v>2.0369999999999999</v>
-      </c>
-      <c r="AE38" s="5">
-        <v>7.7999999999999998</v>
-      </c>
-      <c r="AF38" s="5">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="AG38">
-        <v>223</v>
-      </c>
-      <c r="AH38" s="5">
-        <v>4.5</v>
-      </c>
-      <c r="AI38" s="5">
-        <v>12.1</v>
-      </c>
-      <c r="AJ38" s="5">
-        <v>10.9</v>
-      </c>
-      <c r="AK38" s="3">
-        <v>2.948</v>
-      </c>
-      <c r="AL38" s="3">
-        <v>0.090999999999999998</v>
-      </c>
-      <c r="AM38" s="3">
-        <v>35.561</v>
-      </c>
-      <c r="AN38" s="5">
-        <v>22.699999999999999</v>
-      </c>
-      <c r="AO38" s="5">
-        <v>71.5</v>
-      </c>
-      <c r="AP38" s="4">
-        <v>0.029999999999999999</v>
-      </c>
-      <c r="AQ38" s="3">
-        <v>2.742</v>
-      </c>
-      <c r="AR38" s="4">
-        <v>0.040000000000000001</v>
-      </c>
-      <c r="AS38" s="5">
-        <v>4.7000000000000002</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s">
-        <v>154</v>
-      </c>
-      <c r="B39" t="s">
-        <v>104</v>
-      </c>
-      <c r="C39" t="s">
-        <v>64</v>
-      </c>
-      <c r="D39" t="s">
-        <v>65</v>
-      </c>
-      <c r="E39" s="2">
-        <v>35.062860999999998</v>
-      </c>
-      <c r="F39" s="2">
-        <v>126.772972</v>
-      </c>
-      <c r="G39" t="s">
-        <v>66</v>
-      </c>
-      <c r="H39" t="s">
-        <v>67</v>
-      </c>
-      <c r="L39" t="s">
-        <v>66</v>
-      </c>
-      <c r="M39" t="s">
-        <v>67</v>
-      </c>
-      <c r="N39" t="s">
-        <v>68</v>
-      </c>
-      <c r="O39" t="s">
-        <v>69</v>
-      </c>
-      <c r="P39" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>71</v>
-      </c>
-      <c r="R39" t="s">
-        <v>72</v>
-      </c>
-      <c r="S39" t="s">
-        <v>73</v>
-      </c>
-      <c r="T39" t="s">
-        <v>74</v>
-      </c>
-      <c r="U39" t="s">
-        <v>75</v>
-      </c>
-      <c r="V39" t="s">
-        <v>68</v>
-      </c>
-      <c r="W39" t="s">
-        <v>69</v>
-      </c>
-      <c r="X39" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y39" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z39" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA39" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB39" t="s">
-        <v>155</v>
-      </c>
-      <c r="AC39" s="3">
-        <v>1.2470000000000001</v>
-      </c>
-      <c r="AD39" s="3">
-        <v>1.7729999999999999</v>
-      </c>
-      <c r="AE39" s="5">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="AF39" s="5">
-        <v>13.5</v>
-      </c>
-      <c r="AG39">
-        <v>322</v>
-      </c>
-      <c r="AH39" s="5">
-        <v>6.7999999999999998</v>
-      </c>
-      <c r="AI39" s="5">
-        <v>22.899999999999999</v>
-      </c>
-      <c r="AJ39" s="5">
-        <v>13.5</v>
-      </c>
-      <c r="AK39" s="3">
-        <v>4.1920000000000002</v>
-      </c>
-      <c r="AL39" s="3">
-        <v>0.083000000000000004</v>
-      </c>
-      <c r="AM39" s="3">
-        <v>17.855</v>
-      </c>
-      <c r="AN39" s="5">
-        <v>23.5</v>
-      </c>
-      <c r="AO39" s="5">
-        <v>230.80000000000001</v>
-      </c>
-      <c r="AP39" s="3">
-        <v>0.002</v>
-      </c>
-      <c r="AQ39" s="3">
-        <v>3.9039999999999999</v>
-      </c>
-      <c r="AR39" s="3">
-        <v>0.019</v>
-      </c>
-      <c r="AS39">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40"/>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>